<commit_message>
Adjusts tests to include file paths
</commit_message>
<xml_diff>
--- a/tests/integration_files/get_data expected.xlsx
+++ b/tests/integration_files/get_data expected.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://loreal-my.sharepoint.com/personal/christopher_quartararo_loreal_com/Documents/Documents/Tools (Custom tooling)/Python/Coloshot Automation/tests/integration_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{83E8919F-2D30-4F29-A31F-DBC0ED670373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{114CFCCF-4C23-4879-9D8A-DE21DF95E831}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{83E8919F-2D30-4F29-A31F-DBC0ED670373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2DE52010-6A00-4022-B909-7AC14178C82A}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="28320" xr2:uid="{AF1420F2-F18D-4D3D-8E66-9CB24AB1F74E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="84">
   <si>
     <t>Date</t>
   </si>
@@ -285,6 +285,9 @@
   </si>
   <si>
     <t>20220512-105430</t>
+  </si>
+  <si>
+    <t>File Path</t>
   </si>
 </sst>
 </file>
@@ -636,15 +639,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B33D8B6-ACAD-4027-A591-2635197F6943}">
-  <dimension ref="A1:X27"/>
+  <dimension ref="A1:Y27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Y2" sqref="Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -717,8 +724,11 @@
       <c r="X1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -750,7 +760,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -782,7 +792,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -814,7 +824,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -846,7 +856,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -878,7 +888,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -910,7 +920,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -942,7 +952,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -974,7 +984,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -1006,7 +1016,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>52</v>
       </c>
@@ -1038,7 +1048,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>53</v>
       </c>
@@ -1070,7 +1080,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -1102,7 +1112,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>57</v>
       </c>
@@ -1134,7 +1144,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>60</v>
       </c>
@@ -1166,7 +1176,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>61</v>
       </c>

</xml_diff>